<commit_message>
update files from home pc
</commit_message>
<xml_diff>
--- a/天著湖韵花园-物品收纳表.xlsx
+++ b/天著湖韵花园-物品收纳表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\GitHub_Test_190627\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8667E3-FE76-488F-A232-18A63D692336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF15869-D071-4CD9-B9F0-A5C38B7AA110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BEFFB394-D50D-48DD-85F6-1F4D0567C506}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEFFB394-D50D-48DD-85F6-1F4D0567C506}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="677">
   <si>
     <t>区域编号</t>
   </si>
@@ -962,9 +962,6 @@
   </si>
   <si>
     <t>保温杯</t>
-  </si>
-  <si>
-    <t>黑色，博世</t>
   </si>
   <si>
     <t>普通打火机</t>
@@ -2329,6 +2326,32 @@
   <si>
     <t>白色+咖啡色</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>保温杯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>黑色博世+粉色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>TIGER</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2447,7 +2470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2467,6 +2490,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2795,7 +2820,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2805,17 +2830,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B15" s="18">
         <v>45367</v>
@@ -2823,12 +2848,12 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B17" s="18">
         <v>45367</v>
@@ -2836,7 +2861,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B18" s="18">
         <v>45367</v>
@@ -2853,58 +2878,58 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>659</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -2917,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00AF7DF-ED88-4EBF-B1D5-F94AEE5780DD}">
   <dimension ref="A1:M233"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="M184" sqref="M184"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="I139" sqref="I139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4063,7 +4088,7 @@
         <v>171</v>
       </c>
       <c r="H69" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>3</v>
@@ -5240,7 +5265,7 @@
         <v>5</v>
       </c>
       <c r="K142" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="143" spans="6:12" x14ac:dyDescent="0.2">
@@ -5257,7 +5282,7 @@
         <v>5</v>
       </c>
       <c r="K143" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="144" spans="6:12" x14ac:dyDescent="0.2">
@@ -5274,7 +5299,7 @@
         <v>5</v>
       </c>
       <c r="K144" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="145" spans="6:12" x14ac:dyDescent="0.2">
@@ -5291,7 +5316,7 @@
         <v>5</v>
       </c>
       <c r="K145" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L145" t="s">
         <v>297</v>
@@ -5311,7 +5336,7 @@
         <v>5</v>
       </c>
       <c r="K146" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="147" spans="6:12" x14ac:dyDescent="0.2">
@@ -5331,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="K147" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="148" spans="6:12" x14ac:dyDescent="0.2">
@@ -5348,15 +5373,18 @@
         <v>5</v>
       </c>
       <c r="K148" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="149" spans="6:12" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="149" spans="6:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F149" t="s">
         <v>305</v>
       </c>
-      <c r="H149" t="s">
-        <v>306</v>
+      <c r="G149">
+        <v>2</v>
+      </c>
+      <c r="H149" s="20" t="s">
+        <v>676</v>
       </c>
       <c r="I149" s="3" t="s">
         <v>3</v>
@@ -5365,35 +5393,35 @@
         <v>5</v>
       </c>
       <c r="K149" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="150" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F150" t="s">
+        <v>306</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K150" t="s">
+        <v>326</v>
+      </c>
+      <c r="L150" t="s">
         <v>307</v>
-      </c>
-      <c r="I150" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J150" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K150" t="s">
-        <v>327</v>
-      </c>
-      <c r="L150" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="151" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G151">
         <v>2</v>
       </c>
       <c r="H151" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I151" s="3" t="s">
         <v>3</v>
@@ -5402,19 +5430,19 @@
         <v>5</v>
       </c>
       <c r="K151" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L151" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="152" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F152" t="s">
+        <v>310</v>
+      </c>
+      <c r="H152" t="s">
         <v>311</v>
       </c>
-      <c r="H152" t="s">
-        <v>312</v>
-      </c>
       <c r="I152" s="3" t="s">
         <v>3</v>
       </c>
@@ -5422,19 +5450,19 @@
         <v>5</v>
       </c>
       <c r="K152" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L152" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="153" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F153" t="s">
+        <v>312</v>
+      </c>
+      <c r="H153" t="s">
         <v>313</v>
       </c>
-      <c r="H153" t="s">
-        <v>314</v>
-      </c>
       <c r="I153" s="3" t="s">
         <v>3</v>
       </c>
@@ -5442,15 +5470,15 @@
         <v>5</v>
       </c>
       <c r="K153" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="154" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F154" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H154" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I154" s="3" t="s">
         <v>3</v>
@@ -5459,19 +5487,19 @@
         <v>5</v>
       </c>
       <c r="K154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="156" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F156" t="s">
+        <v>317</v>
+      </c>
+      <c r="G156">
+        <v>3</v>
+      </c>
+      <c r="H156" t="s">
         <v>318</v>
       </c>
-      <c r="G156">
-        <v>3</v>
-      </c>
-      <c r="H156" t="s">
-        <v>319</v>
-      </c>
       <c r="I156" s="3" t="s">
         <v>3</v>
       </c>
@@ -5479,15 +5507,15 @@
         <v>5</v>
       </c>
       <c r="K156" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="157" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F157" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H157" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I157" s="3" t="s">
         <v>3</v>
@@ -5496,18 +5524,18 @@
         <v>5</v>
       </c>
       <c r="K157" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="158" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G158">
         <v>4</v>
       </c>
       <c r="H158" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>3</v>
@@ -5516,16 +5544,16 @@
         <v>5</v>
       </c>
       <c r="K158" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="159" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F159" t="s">
+        <v>323</v>
+      </c>
+      <c r="H159" t="s">
         <v>324</v>
       </c>
-      <c r="H159" t="s">
-        <v>325</v>
-      </c>
       <c r="I159" s="3" t="s">
         <v>3</v>
       </c>
@@ -5533,12 +5561,12 @@
         <v>5</v>
       </c>
       <c r="K159" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="160" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F160" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>3</v>
@@ -5547,7 +5575,7 @@
         <v>5</v>
       </c>
       <c r="K160" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="161" spans="6:12" x14ac:dyDescent="0.2">
@@ -5564,7 +5592,7 @@
         <v>5</v>
       </c>
       <c r="K161" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L161" t="s">
         <v>297</v>
@@ -5572,11 +5600,11 @@
     </row>
     <row r="162" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F162" t="s">
+        <v>328</v>
+      </c>
+      <c r="H162" t="s">
         <v>329</v>
       </c>
-      <c r="H162" t="s">
-        <v>330</v>
-      </c>
       <c r="I162" s="3" t="s">
         <v>3</v>
       </c>
@@ -5584,15 +5612,15 @@
         <v>5</v>
       </c>
       <c r="K162" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="163" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F163" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H163" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I163" s="3" t="s">
         <v>3</v>
@@ -5601,12 +5629,12 @@
         <v>5</v>
       </c>
       <c r="K163" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="164" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F164" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I164" s="3" t="s">
         <v>3</v>
@@ -5615,12 +5643,12 @@
         <v>5</v>
       </c>
       <c r="K164" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="165" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F165" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I165" s="3" t="s">
         <v>3</v>
@@ -5629,18 +5657,18 @@
         <v>5</v>
       </c>
       <c r="K165" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="166" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F166" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G166">
         <v>2</v>
       </c>
       <c r="H166" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I166" s="3" t="s">
         <v>3</v>
@@ -5649,16 +5677,16 @@
         <v>5</v>
       </c>
       <c r="K166" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="167" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F167" t="s">
+        <v>336</v>
+      </c>
+      <c r="H167" t="s">
         <v>337</v>
       </c>
-      <c r="H167" t="s">
-        <v>338</v>
-      </c>
       <c r="I167" s="3" t="s">
         <v>3</v>
       </c>
@@ -5666,18 +5694,18 @@
         <v>5</v>
       </c>
       <c r="K167" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="168" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F168" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G168">
         <v>8</v>
       </c>
       <c r="H168" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I168" s="3" t="s">
         <v>3</v>
@@ -5686,16 +5714,16 @@
         <v>5</v>
       </c>
       <c r="K168" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="170" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F170" t="s">
+        <v>339</v>
+      </c>
+      <c r="H170" t="s">
         <v>340</v>
       </c>
-      <c r="H170" t="s">
-        <v>341</v>
-      </c>
       <c r="I170" s="3" t="s">
         <v>3</v>
       </c>
@@ -5703,33 +5731,33 @@
         <v>5</v>
       </c>
       <c r="K170" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="171" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F171" t="s">
+        <v>341</v>
+      </c>
+      <c r="H171" t="s">
+        <v>346</v>
+      </c>
+      <c r="I171" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J171" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K171" t="s">
         <v>342</v>
-      </c>
-      <c r="H171" t="s">
-        <v>347</v>
-      </c>
-      <c r="I171" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J171" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K171" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="172" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F172" t="s">
+        <v>344</v>
+      </c>
+      <c r="H172" t="s">
         <v>345</v>
       </c>
-      <c r="H172" t="s">
-        <v>346</v>
-      </c>
       <c r="I172" s="3" t="s">
         <v>3</v>
       </c>
@@ -5737,33 +5765,33 @@
         <v>5</v>
       </c>
       <c r="K172" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="173" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F173" t="s">
+        <v>347</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K173" t="s">
+        <v>343</v>
+      </c>
+      <c r="L173" t="s">
         <v>348</v>
-      </c>
-      <c r="I173" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J173" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K173" t="s">
-        <v>344</v>
-      </c>
-      <c r="L173" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="174" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F174" t="s">
+        <v>349</v>
+      </c>
+      <c r="H174" t="s">
         <v>350</v>
       </c>
-      <c r="H174" t="s">
-        <v>351</v>
-      </c>
       <c r="I174" s="3" t="s">
         <v>3</v>
       </c>
@@ -5771,12 +5799,12 @@
         <v>5</v>
       </c>
       <c r="K174" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="175" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F175" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I175" s="3" t="s">
         <v>3</v>
@@ -5785,12 +5813,12 @@
         <v>5</v>
       </c>
       <c r="K175" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="176" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F176" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I176" s="3" t="s">
         <v>3</v>
@@ -5799,12 +5827,12 @@
         <v>5</v>
       </c>
       <c r="K176" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="177" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F177" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G177">
         <v>3</v>
@@ -5816,18 +5844,18 @@
         <v>5</v>
       </c>
       <c r="K177" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="178" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F178" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G178">
         <v>2</v>
       </c>
       <c r="H178" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I178" s="3" t="s">
         <v>3</v>
@@ -5836,12 +5864,12 @@
         <v>5</v>
       </c>
       <c r="K178" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="179" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F179" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I179" s="3" t="s">
         <v>3</v>
@@ -5850,18 +5878,18 @@
         <v>5</v>
       </c>
       <c r="K179" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L179" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="180" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F180" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H180" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I180" s="3" t="s">
         <v>3</v>
@@ -5870,12 +5898,12 @@
         <v>5</v>
       </c>
       <c r="K180" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="181" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F181" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I181" s="3" t="s">
         <v>3</v>
@@ -5884,15 +5912,15 @@
         <v>5</v>
       </c>
       <c r="K181" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="182" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F182" t="s">
-        <v>305</v>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="182" spans="6:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="F182" s="19" t="s">
+        <v>675</v>
       </c>
       <c r="H182" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I182" s="3" t="s">
         <v>3</v>
@@ -5901,16 +5929,16 @@
         <v>5</v>
       </c>
       <c r="K182" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="183" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F183" t="s">
+        <v>359</v>
+      </c>
+      <c r="H183" t="s">
         <v>360</v>
       </c>
-      <c r="H183" t="s">
-        <v>361</v>
-      </c>
       <c r="I183" s="3" t="s">
         <v>3</v>
       </c>
@@ -5918,39 +5946,39 @@
         <v>5</v>
       </c>
       <c r="K183" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="184" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F184" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H184" t="s">
+        <v>362</v>
+      </c>
+      <c r="I184" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J184" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K184" t="s">
+        <v>343</v>
+      </c>
+      <c r="L184" t="s">
         <v>363</v>
       </c>
-      <c r="I184" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J184" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K184" t="s">
-        <v>344</v>
-      </c>
-      <c r="L184" t="s">
+      <c r="M184" t="s">
         <v>364</v>
-      </c>
-      <c r="M184" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="185" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F185" t="s">
+        <v>365</v>
+      </c>
+      <c r="H185" t="s">
         <v>366</v>
       </c>
-      <c r="H185" t="s">
-        <v>367</v>
-      </c>
       <c r="I185" s="3" t="s">
         <v>3</v>
       </c>
@@ -5958,15 +5986,15 @@
         <v>5</v>
       </c>
       <c r="K185" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L185" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="186" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F186" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I186" s="3" t="s">
         <v>3</v>
@@ -5975,12 +6003,12 @@
         <v>5</v>
       </c>
       <c r="K186" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="187" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F187" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I187" s="3" t="s">
         <v>3</v>
@@ -5989,12 +6017,12 @@
         <v>5</v>
       </c>
       <c r="K187" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="188" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F188" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I188" s="3" t="s">
         <v>3</v>
@@ -6003,12 +6031,12 @@
         <v>5</v>
       </c>
       <c r="K188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="190" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F190" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I190" s="3" t="s">
         <v>3</v>
@@ -6017,16 +6045,16 @@
         <v>5</v>
       </c>
       <c r="K190" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="191" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F191" t="s">
+        <v>372</v>
+      </c>
+      <c r="H191" t="s">
         <v>373</v>
       </c>
-      <c r="H191" t="s">
-        <v>374</v>
-      </c>
       <c r="I191" s="3" t="s">
         <v>3</v>
       </c>
@@ -6034,15 +6062,15 @@
         <v>5</v>
       </c>
       <c r="K191" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="192" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F192" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H192" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I192" s="3" t="s">
         <v>3</v>
@@ -6051,15 +6079,15 @@
         <v>5</v>
       </c>
       <c r="K192" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="193" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F193" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H193" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I193" s="3" t="s">
         <v>3</v>
@@ -6068,16 +6096,16 @@
         <v>5</v>
       </c>
       <c r="K193" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="194" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F194" t="s">
+        <v>377</v>
+      </c>
+      <c r="H194" t="s">
         <v>378</v>
       </c>
-      <c r="H194" t="s">
-        <v>379</v>
-      </c>
       <c r="I194" s="3" t="s">
         <v>3</v>
       </c>
@@ -6085,12 +6113,12 @@
         <v>5</v>
       </c>
       <c r="K194" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="195" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F195" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I195" s="3" t="s">
         <v>3</v>
@@ -6099,18 +6127,18 @@
         <v>5</v>
       </c>
       <c r="K195" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="196" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F196" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G196">
         <v>2</v>
       </c>
       <c r="H196" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I196" s="3" t="s">
         <v>3</v>
@@ -6119,12 +6147,12 @@
         <v>5</v>
       </c>
       <c r="K196" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="197" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F197" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I197" s="3" t="s">
         <v>3</v>
@@ -6133,7 +6161,7 @@
         <v>5</v>
       </c>
       <c r="K197" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="198" spans="6:12" x14ac:dyDescent="0.2">
@@ -6147,7 +6175,7 @@
         <v>5</v>
       </c>
       <c r="K198" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L198" s="7" t="s">
         <v>233</v>
@@ -6155,7 +6183,7 @@
     </row>
     <row r="199" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F199" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I199" s="3" t="s">
         <v>3</v>
@@ -6164,7 +6192,7 @@
         <v>5</v>
       </c>
       <c r="K199" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L199" s="7" t="s">
         <v>233</v>
@@ -6172,7 +6200,7 @@
     </row>
     <row r="200" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F200" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I200" s="3" t="s">
         <v>3</v>
@@ -6181,7 +6209,7 @@
         <v>5</v>
       </c>
       <c r="K200" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L200" s="7" t="s">
         <v>233</v>
@@ -6195,7 +6223,7 @@
         <v>5</v>
       </c>
       <c r="K201" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L201" s="7" t="s">
         <v>233</v>
@@ -6203,7 +6231,7 @@
     </row>
     <row r="203" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F203" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I203" s="3" t="s">
         <v>3</v>
@@ -6212,12 +6240,12 @@
         <v>7</v>
       </c>
       <c r="K203" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="204" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F204" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I204" s="3" t="s">
         <v>3</v>
@@ -6226,15 +6254,15 @@
         <v>7</v>
       </c>
       <c r="K204" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="205" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F205" t="s">
+        <v>389</v>
+      </c>
+      <c r="H205" t="s">
         <v>390</v>
-      </c>
-      <c r="H205" t="s">
-        <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
         <v>3</v>
@@ -6243,15 +6271,15 @@
         <v>7</v>
       </c>
       <c r="K205" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="206" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F206" t="s">
+        <v>391</v>
+      </c>
+      <c r="H206" t="s">
         <v>392</v>
-      </c>
-      <c r="H206" t="s">
-        <v>393</v>
       </c>
       <c r="I206" s="3" t="s">
         <v>3</v>
@@ -6260,15 +6288,15 @@
         <v>7</v>
       </c>
       <c r="K206" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="207" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F207" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H207" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I207" t="s">
         <v>17</v>
@@ -6279,13 +6307,13 @@
     </row>
     <row r="208" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F208" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G208">
         <v>1</v>
       </c>
       <c r="H208" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I208" s="3" t="s">
         <v>3</v>
@@ -6294,18 +6322,18 @@
         <v>7</v>
       </c>
       <c r="K208" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="209" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F209" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G209">
         <v>1</v>
       </c>
       <c r="H209" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I209" s="3" t="s">
         <v>3</v>
@@ -6314,12 +6342,12 @@
         <v>7</v>
       </c>
       <c r="K209" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="210" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F210" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I210" s="3" t="s">
         <v>3</v>
@@ -6328,18 +6356,18 @@
         <v>7</v>
       </c>
       <c r="K210" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="211" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F211" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G211">
         <v>2</v>
       </c>
       <c r="H211" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I211" s="3" t="s">
         <v>3</v>
@@ -6348,15 +6376,15 @@
         <v>7</v>
       </c>
       <c r="K211" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="212" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F212" t="s">
+        <v>401</v>
+      </c>
+      <c r="H212" t="s">
         <v>402</v>
-      </c>
-      <c r="H212" t="s">
-        <v>403</v>
       </c>
       <c r="I212" s="3" t="s">
         <v>3</v>
@@ -6365,18 +6393,18 @@
         <v>7</v>
       </c>
       <c r="K212" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="213" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F213" t="s">
+        <v>403</v>
+      </c>
+      <c r="G213">
+        <v>3</v>
+      </c>
+      <c r="H213" t="s">
         <v>404</v>
-      </c>
-      <c r="G213">
-        <v>3</v>
-      </c>
-      <c r="H213" t="s">
-        <v>405</v>
       </c>
       <c r="I213" s="3" t="s">
         <v>3</v>
@@ -6385,12 +6413,12 @@
         <v>7</v>
       </c>
       <c r="K213" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="214" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F214" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I214" s="3" t="s">
         <v>3</v>
@@ -6399,15 +6427,15 @@
         <v>7</v>
       </c>
       <c r="K214" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="215" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F215" t="s">
+        <v>387</v>
+      </c>
+      <c r="H215" t="s">
         <v>388</v>
-      </c>
-      <c r="H215" t="s">
-        <v>389</v>
       </c>
       <c r="I215" s="3" t="s">
         <v>3</v>
@@ -6421,7 +6449,7 @@
     </row>
     <row r="216" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F216" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H216" t="s">
         <v>191</v>
@@ -6438,10 +6466,10 @@
     </row>
     <row r="217" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F217" t="s">
+        <v>406</v>
+      </c>
+      <c r="H217" t="s">
         <v>407</v>
-      </c>
-      <c r="H217" t="s">
-        <v>408</v>
       </c>
       <c r="I217" s="3" t="s">
         <v>3</v>
@@ -6455,10 +6483,10 @@
     </row>
     <row r="218" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F218" t="s">
+        <v>411</v>
+      </c>
+      <c r="H218" t="s">
         <v>412</v>
-      </c>
-      <c r="H218" t="s">
-        <v>413</v>
       </c>
       <c r="I218" s="3" t="s">
         <v>3</v>
@@ -6472,7 +6500,7 @@
     </row>
     <row r="219" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F219" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I219" s="8" t="s">
         <v>3</v>
@@ -6486,13 +6514,13 @@
     </row>
     <row r="233" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F233" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="I233" s="10" t="s">
         <v>648</v>
       </c>
-      <c r="I233" s="10" t="s">
+      <c r="L233" s="11" t="s">
         <v>649</v>
-      </c>
-      <c r="L233" s="11" t="s">
-        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -6518,7 +6546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368D5EFC-7084-4DE3-B0BC-447396EE266E}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
@@ -6579,10 +6607,10 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6597,10 +6625,10 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="8"/>
@@ -6615,10 +6643,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="8"/>
@@ -6633,10 +6661,10 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6651,7 +6679,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -6671,7 +6699,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -6691,16 +6719,16 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>423</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>424</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -6711,7 +6739,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -6720,7 +6748,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -6731,7 +6759,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -6740,7 +6768,7 @@
         <v>25</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -6751,16 +6779,16 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -6771,16 +6799,16 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -6791,13 +6819,13 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>23</v>
@@ -6811,7 +6839,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -6820,7 +6848,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -6831,7 +6859,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -6840,7 +6868,7 @@
         <v>17</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -6851,7 +6879,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -6860,7 +6888,7 @@
         <v>25</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -6870,19 +6898,19 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G17" s="3">
         <v>2</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -6894,19 +6922,19 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G18" s="3">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -6918,13 +6946,13 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G19" s="3">
         <v>14</v>
@@ -6944,22 +6972,22 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G20" s="3">
         <v>8</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -6970,13 +6998,13 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G21" s="3">
         <v>3</v>
@@ -6990,7 +7018,7 @@
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -6998,19 +7026,19 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>17</v>
@@ -7020,7 +7048,7 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -7028,13 +7056,13 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G23" s="3">
         <v>1</v>
@@ -7054,19 +7082,19 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G24" s="3">
         <v>5</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>17</v>
@@ -7082,25 +7110,25 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -7108,25 +7136,25 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G26" s="3">
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -7134,13 +7162,13 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G27" s="3">
         <v>1</v>
@@ -7152,7 +7180,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -7160,13 +7188,13 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G28" s="3">
         <v>1</v>
@@ -7176,7 +7204,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -7184,22 +7212,22 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G29" s="3">
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>461</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>462</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -7210,19 +7238,19 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G30" s="3">
         <v>3</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -7234,19 +7262,19 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>516</v>
-      </c>
-      <c r="G31" s="3">
-        <v>3</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>517</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>17</v>
@@ -7262,19 +7290,19 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G32" s="3">
         <v>2</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>17</v>
@@ -7288,25 +7316,25 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G33" s="3">
         <v>1</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="16" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -7314,19 +7342,19 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G34" s="3">
         <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -7338,25 +7366,25 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G35" s="3">
         <v>4</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -7364,25 +7392,25 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="G36" s="3">
-        <v>3</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>540</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -7390,25 +7418,25 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E37" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>643</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>644</v>
       </c>
       <c r="G37" s="3">
         <v>2</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -7416,25 +7444,25 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E38" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>643</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>644</v>
       </c>
       <c r="G38" s="3">
         <v>4</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -7445,16 +7473,16 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G39" s="3">
         <v>1</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>17</v>
@@ -7463,7 +7491,7 @@
         <v>19</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="L39" s="3"/>
     </row>
@@ -7473,16 +7501,16 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G40" s="3">
         <v>2</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>17</v>
@@ -7499,14 +7527,14 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>17</v>
@@ -7523,16 +7551,16 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G42" s="3">
         <v>1</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>17</v>
@@ -7548,29 +7576,29 @@
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G43" s="3">
         <v>1</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I43" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="J43" s="12" t="s">
         <v>591</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>592</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -7578,29 +7606,29 @@
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I44" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="J44" s="12" t="s">
         <v>591</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>592</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -7608,29 +7636,29 @@
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E45" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="F45" s="12" t="s">
         <v>589</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>590</v>
       </c>
       <c r="G45" s="3">
         <v>2</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I45" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="J45" s="12" t="s">
         <v>591</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>592</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -7638,19 +7666,19 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G46" s="3">
         <v>2</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -7662,19 +7690,19 @@
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G47" s="3">
         <v>2</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>17</v>
@@ -7690,29 +7718,29 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G48" s="3">
         <v>3</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -7720,27 +7748,27 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G49" s="3">
         <v>1</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="3"/>
       <c r="L49" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -7748,19 +7776,19 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G50" s="3">
         <v>2</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>17</v>
@@ -7770,7 +7798,7 @@
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -7778,19 +7806,19 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G51" s="3">
         <v>3</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>17</v>
@@ -7806,19 +7834,19 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G52" s="3">
         <v>1</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>17</v>
@@ -7834,19 +7862,19 @@
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G53" s="3">
         <v>1</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>17</v>
@@ -7862,19 +7890,19 @@
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G54" s="3">
         <v>2</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>17</v>
@@ -7890,22 +7918,22 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G55" s="3">
         <v>1</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -7916,22 +7944,22 @@
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G56" s="3">
         <v>1</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -7942,22 +7970,22 @@
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G57" s="3">
         <v>1</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -7968,13 +7996,13 @@
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G58" s="3">
         <v>1</v>
@@ -7994,28 +8022,28 @@
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G59" s="3">
         <v>1</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L59" s="3"/>
     </row>
@@ -8024,13 +8052,13 @@
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -8048,19 +8076,19 @@
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G61" s="3">
         <v>2</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>17</v>
@@ -8076,19 +8104,19 @@
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G62" s="3">
         <v>19</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>17</v>
@@ -8098,7 +8126,7 @@
       </c>
       <c r="K62" s="3"/>
       <c r="L62" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -8106,13 +8134,13 @@
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G63" s="3">
         <v>11</v>
@@ -8132,19 +8160,19 @@
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G64" s="3">
         <v>1</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>17</v>
@@ -8160,25 +8188,25 @@
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G65" s="3">
         <v>1</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -8186,19 +8214,19 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G66" s="3">
         <v>2</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -8210,13 +8238,13 @@
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F67" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G67" s="3">
         <v>5</v>
@@ -8232,7 +8260,7 @@
       </c>
       <c r="K67" s="3"/>
       <c r="L67" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -8240,19 +8268,19 @@
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F68" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G68" s="3">
         <v>3</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>17</v>
@@ -8262,7 +8290,7 @@
       </c>
       <c r="K68" s="3"/>
       <c r="L68" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -8270,19 +8298,19 @@
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F69" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G69" s="3">
         <v>4</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>17</v>
@@ -8296,19 +8324,19 @@
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F70" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G70" s="3">
         <v>2</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>17</v>
@@ -8322,19 +8350,19 @@
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F71" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G71" s="3">
         <v>1</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>17</v>
@@ -8350,19 +8378,19 @@
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F72" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G72" s="3">
         <v>1</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>17</v>
@@ -8378,13 +8406,13 @@
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F73" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G73" s="3">
         <v>8</v>
@@ -8400,19 +8428,19 @@
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F74" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G74" s="3">
         <v>1</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -8424,19 +8452,19 @@
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F75" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G75" s="3">
         <v>2</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
@@ -8448,19 +8476,19 @@
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F76" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G76" s="3">
         <v>2</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>17</v>
@@ -8476,13 +8504,13 @@
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F77" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G77" s="3">
         <v>2</v>
@@ -8502,19 +8530,19 @@
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F78" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G78" s="3">
         <v>2</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>17</v>
@@ -8530,22 +8558,22 @@
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F79" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G79" s="3">
         <v>1</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -8556,19 +8584,19 @@
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>549</v>
-      </c>
       <c r="F80" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G80" s="3">
         <v>2</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>17</v>
@@ -8584,19 +8612,19 @@
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G81" s="3">
         <v>1</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
@@ -8608,19 +8636,19 @@
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G82" s="3">
         <v>4</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
@@ -8632,13 +8660,13 @@
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -8652,13 +8680,13 @@
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -8672,19 +8700,19 @@
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G85" s="3">
         <v>1</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
@@ -8696,29 +8724,29 @@
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G86" s="3">
         <v>2</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K86" s="3"/>
       <c r="L86" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -8726,25 +8754,25 @@
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G87" s="3">
         <v>1</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K87" s="3"/>
       <c r="L87" s="12"/>
@@ -8754,25 +8782,25 @@
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G88" s="3">
         <v>1</v>
       </c>
       <c r="H88" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="I88" s="12" t="s">
         <v>603</v>
       </c>
-      <c r="I88" s="12" t="s">
+      <c r="J88" s="12" t="s">
         <v>604</v>
-      </c>
-      <c r="J88" s="12" t="s">
-        <v>605</v>
       </c>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
@@ -8782,19 +8810,19 @@
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F89" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="G89" s="3">
+        <v>3</v>
+      </c>
+      <c r="H89" s="12" t="s">
         <v>606</v>
-      </c>
-      <c r="G89" s="3">
-        <v>3</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>607</v>
       </c>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
@@ -8806,19 +8834,19 @@
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G90" s="3">
         <v>2</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -8830,19 +8858,19 @@
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G91" s="3">
         <v>2</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
@@ -8854,19 +8882,19 @@
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G92" s="3">
         <v>1</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>17</v>
@@ -8882,19 +8910,19 @@
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G93" s="3">
         <v>2</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>17</v>
@@ -8910,19 +8938,19 @@
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G94" s="3">
         <v>3</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
@@ -8934,17 +8962,17 @@
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I95" s="3" t="s">
         <v>17</v>
@@ -8960,17 +8988,17 @@
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I96" s="3" t="s">
         <v>17</v>
@@ -8986,19 +9014,19 @@
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G97" s="3">
         <v>1</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I97" s="3" t="s">
         <v>1</v>
@@ -9006,7 +9034,7 @@
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
@@ -9014,19 +9042,19 @@
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G98" s="3">
         <v>1</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
@@ -9038,19 +9066,19 @@
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G99" s="3">
         <v>1</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>17</v>
@@ -9066,19 +9094,19 @@
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G100" s="3">
         <v>1</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>17</v>
@@ -9092,25 +9120,25 @@
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G101" s="3">
         <v>1</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
@@ -9118,25 +9146,25 @@
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G102" s="3">
         <v>9</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
@@ -9144,19 +9172,19 @@
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G103" s="3">
         <v>4</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I103" s="3" t="s">
         <v>1</v>
@@ -9170,19 +9198,19 @@
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F104" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G104" s="3">
+        <v>3</v>
+      </c>
+      <c r="H104" s="3" t="s">
         <v>474</v>
-      </c>
-      <c r="G104" s="3">
-        <v>3</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>475</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>17</v>
@@ -9192,7 +9220,7 @@
       </c>
       <c r="K104" s="3"/>
       <c r="L104" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
@@ -9200,19 +9228,19 @@
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G105" s="3">
         <v>2</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I105" s="3" t="s">
         <v>17</v>
@@ -9222,7 +9250,7 @@
       </c>
       <c r="K105" s="3"/>
       <c r="L105" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
@@ -9230,19 +9258,19 @@
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G106" s="3">
         <v>4</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I106" s="3" t="s">
         <v>17</v>
@@ -9259,22 +9287,22 @@
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G107" s="3">
         <v>4</v>
       </c>
       <c r="H107" s="12" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I107" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J107" s="13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
@@ -9285,22 +9313,22 @@
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G108" s="3">
         <v>2</v>
       </c>
       <c r="H108" s="12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I108" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
@@ -9311,22 +9339,22 @@
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F109" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="G109" s="3">
+        <v>3</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>615</v>
+      </c>
+      <c r="I109" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="J109" s="13" t="s">
         <v>613</v>
-      </c>
-      <c r="G109" s="3">
-        <v>3</v>
-      </c>
-      <c r="H109" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="I109" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="J109" s="13" t="s">
-        <v>614</v>
       </c>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
@@ -9337,24 +9365,24 @@
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F110" s="12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G110" s="3">
         <v>3</v>
       </c>
       <c r="H110" s="12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I110" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J110" s="13"/>
       <c r="K110" s="3"/>
       <c r="L110" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
@@ -9363,19 +9391,19 @@
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F111" s="12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G111" s="3">
         <v>2</v>
       </c>
       <c r="H111" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I111" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
@@ -9387,19 +9415,19 @@
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F112" s="12" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G112" s="3">
         <v>1</v>
       </c>
       <c r="H112" s="12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I112" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
@@ -9411,19 +9439,19 @@
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G113" s="3">
         <v>1</v>
       </c>
       <c r="H113" s="12" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I113" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
@@ -9435,16 +9463,16 @@
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F114" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="G114" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H114" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
@@ -9457,22 +9485,22 @@
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G115" s="3">
         <v>1</v>
       </c>
       <c r="H115" s="12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I115" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J115" s="13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
@@ -9497,20 +9525,20 @@
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G117" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="J117" s="12" t="s">
         <v>672</v>
-      </c>
-      <c r="J117" s="12" t="s">
-        <v>673</v>
       </c>
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
@@ -9521,22 +9549,22 @@
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G118" s="3">
         <v>2</v>
       </c>
       <c r="H118" s="12" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I118" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J118" s="12" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>

</xml_diff>